<commit_message>
suppression de keywords dans les 2pages
</commit_message>
<xml_diff>
--- a/Modèle-audit-SEO.xlsx
+++ b/Modèle-audit-SEO.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Catégorie</t>
   </si>
@@ -54,9 +54,6 @@
   </si>
   <si>
     <t>Performance</t>
-  </si>
-  <si>
-    <t>P1</t>
   </si>
   <si>
     <t>Placez la déclaration doctype en tête de votre fichier HTML, juste après l'ouverture de la balise &lt;html&gt;.
@@ -88,12 +85,47 @@
       <t>(2récurence sur la page Index.html et Page2.html)</t>
     </r>
   </si>
+  <si>
+    <t xml:space="preserve">A FAIRE </t>
+  </si>
+  <si>
+    <t>La balise meta "keywords" était utilisée autrefois pour indiquer aux moteurs de recherche les mots-clés associés à une page web. Cependant, cette balise est devenue obsolète et n'est plus prise en compte par les moteurs de recherche, notamment Google, qui ne l'utilise plus depuis 2009. Il est donc inutile de l'utiliser dans votre code HTML.</t>
+  </si>
+  <si>
+    <t>pour améliorer la référence du site on va plutôt utiliser d'autres éléments tels que le contenu de qualité, la structure du site et les balises meta "description" et "title</t>
+  </si>
+  <si>
+    <t>https://www.balisemeta.com/raison-du-declin-balise-keywords.html</t>
+  </si>
+  <si>
+    <r>
+      <t>La balise meta "keywords" est obsolète et ne devrait pas être utilisée</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">(2récurence sur la page Index.html et Page2.html) </t>
+    </r>
+  </si>
+  <si>
+    <t>Autre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">remplacer par ?&lt;meta name="robots" content="index, follow"&gt;  </t>
+  </si>
+  <si>
+    <t>compléter les balise (qui sont mal utlisé dans le site) en utilisant mieux les balises "description" et "title".Suppression de la ligne sur les 2 pages</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -160,8 +192,14 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -177,6 +215,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -201,7 +245,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -235,6 +279,12 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -455,7 +505,7 @@
   <dimension ref="A1:AA1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.26953125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -464,7 +514,7 @@
     <col min="2" max="2" width="9.81640625" style="6" customWidth="1"/>
     <col min="3" max="3" width="32.1796875" style="6" customWidth="1"/>
     <col min="4" max="4" width="58.54296875" style="6" customWidth="1"/>
-    <col min="5" max="5" width="26.1796875" style="6" customWidth="1"/>
+    <col min="5" max="5" width="24.81640625" style="6" customWidth="1"/>
     <col min="6" max="6" width="14.453125" style="6" customWidth="1"/>
     <col min="7" max="7" width="11.81640625" style="6" customWidth="1"/>
     <col min="8" max="27" width="10.54296875" style="6" customWidth="1"/>
@@ -493,7 +543,9 @@
       <c r="G1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="5"/>
+      <c r="H1" s="13" t="s">
+        <v>18</v>
+      </c>
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
       <c r="K1" s="5"/>
@@ -515,31 +567,53 @@
       <c r="AA1" s="5"/>
     </row>
     <row r="2" spans="1:27" ht="172.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>8</v>
+      <c r="A2" s="1">
+        <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" ht="120" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="6">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" s="10" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="1"/>
-      <c r="F3" s="7"/>
+      <c r="C3" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="4" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F4" s="7"/>
@@ -1565,8 +1639,9 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G2" r:id="rId1"/>
+    <hyperlink ref="G3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape" r:id="rId2"/>
+  <pageSetup orientation="landscape" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Ajout de 8 nouvelles erreurs découvert dans le validateur html et css
meta "keywords",balise <li>,eurrer d'écriture pour la balise<html lang="Default">,Pas de titre, / ,obsolète min-device-width ,obsolète max-device-width
</commit_message>
<xml_diff>
--- a/Modèle-audit-SEO.xlsx
+++ b/Modèle-audit-SEO.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="44">
   <si>
     <t>Catégorie</t>
   </si>
@@ -86,9 +86,6 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">A FAIRE </t>
-  </si>
-  <si>
     <t>La balise meta "keywords" était utilisée autrefois pour indiquer aux moteurs de recherche les mots-clés associés à une page web. Cependant, cette balise est devenue obsolète et n'est plus prise en compte par les moteurs de recherche, notamment Google, qui ne l'utilise plus depuis 2009. Il est donc inutile de l'utiliser dans votre code HTML.</t>
   </si>
   <si>
@@ -120,12 +117,129 @@
   <si>
     <t>compléter les balise (qui sont mal utlisé dans le site) en utilisant mieux les balises "description" et "title".Suppression de la ligne sur les 2 pages</t>
   </si>
+  <si>
+    <t xml:space="preserve">SEO </t>
+  </si>
+  <si>
+    <t>Il y a une balise &lt;li&gt; inutile à la ligne 50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">La balise &lt;li&gt; inutile à la ligne 50 est inutile car elle ne contient aucun contenu ni aucune autre balise enfant. Cela peut causer des erreurs de validation et de rendu de la page. </t>
+  </si>
+  <si>
+    <t>Il est donc recommandé de supprimer cette balise pour éviter tout problème de rendu ou de validation.</t>
+  </si>
+  <si>
+    <t>https://developer.mozilla.org/fr/docs/Web/HTML/Element/li</t>
+  </si>
+  <si>
+    <t>Il est recommandé de mettre un code valide pour l'attribut "lang" dans la balise &lt;html&gt; pour spécifier la langue utilisée pour la page web. Cela permet aux navigateurs et aux utilisateurs de comprendre dans quelle langue est écrite la page et de l'afficher correctement. Il est important de faire cela car cela contribue à une meilleure compatibilité et une meilleure accessibilité pour les utilisateurs qui visitent votre site.</t>
+  </si>
+  <si>
+    <t>mettre la langue principale de la page "fr". Cela contribue à une meilleure compatibilité et une meilleure accessibilité pour les utilisateurs qui visitent votre site.&lt;html lang="fr"&gt;</t>
+  </si>
+  <si>
+    <t>https://www.w3.org/International/questions/qa-html-language-declarations</t>
+  </si>
+  <si>
+    <t>pour le titre la balise est écrit "&lt;title&gt;.&lt;/title&gt;" Il est important de mettre un titre valide et pertinent pour la page dans la balise &lt;title&gt; car cela permet aux utilisateurs et aux moteurs de recherche de comprendre le sujet de votre page, cela améliore l'expérience utilisateur et cela aide à être bien référencé dans les résultats de recherche.</t>
+  </si>
+  <si>
+    <t>La bonne pratique pour la balise &lt;title&gt; est de mettre un titre valide, pertinent et descriptif pour la page. Il doit être court, précis et refléter le contenu de la page. Il est important de ne pas utiliser de mots clés inutiles ou de répéter plusieurs fois le même mot-clé. Il est également important de s'assurer que chaque page de votre site a un titre unique, et qu'il est différent des autres pages pour éviter la duplication de contenu.</t>
+  </si>
+  <si>
+    <t>https://www.search-factory.fr/balise-title/</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Pas de titre </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">(2récurence sur la page Index.html et Page2.html) </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>eurrer d'écriture pour la balise                   &lt;html lang="Default"&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">(2récurence sur la page Index.html et Page2.html) </t>
+    </r>
+  </si>
+  <si>
+    <t>il faut écrit plutôt comme ça &lt;img src="img/agence-la-panthere-monochrome.svg" alt="paris web design logo agence web meilleure agence" height="40" /&gt;</t>
+  </si>
+  <si>
+    <t>Utiliser un slash à la fin d'une balise vide peut causer des erreurs de rendu ou des problèmes de compatibilité avec certains navigateurs ou outils de développement.
+Cela peut également causer des problèmes d'accessibilité pour les utilisateurs d'assistive technologie qui peuvent ne pas être capables de comprendre correctement le contenu de la page.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">/ ajouté en trop </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">(13récurence sur la page Index.html et Page2.html) </t>
+    </r>
+  </si>
+  <si>
+    <t>il y a un attribut 'success-msg' et 'fail-msg' qui ne sont pas autorisés pour l'élément 'form' dans le code HTML. Ces attributs ne font pas partie des attributs standard de la balise 'form' définis par la norme HTML.</t>
+  </si>
+  <si>
+    <t>Il est préférable d'utiliser la balise "form" avec l'attribut "novalidate" plutôt que d'utiliser des attributs personnalisés, car cela est conforme aux normes de développement web et est pris en charge par tous les navigateurs.                                                                                       Ça donnerai : &lt;form id="form_1" novalidate&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eurre avec la balise from </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Performance </t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>https://developer.mozilla.org/fr/docs/Web/HTML/Element/form</t>
+  </si>
+  <si>
+    <t>https://www.alsacreations.com/article/lire/1407-balises-vides-auto-fermantes-en-html.html</t>
+  </si>
+  <si>
+    <r>
+      <t>média obsolète min-device-width (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>2récurence dans le style.css)</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -163,12 +277,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color theme="0"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
@@ -196,6 +304,19 @@
       <b/>
       <sz val="12"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -243,17 +364,14 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -268,23 +386,32 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -504,67 +631,67 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.26953125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.453125" style="6" customWidth="1"/>
-    <col min="2" max="2" width="9.81640625" style="6" customWidth="1"/>
-    <col min="3" max="3" width="32.1796875" style="6" customWidth="1"/>
-    <col min="4" max="4" width="58.54296875" style="6" customWidth="1"/>
-    <col min="5" max="5" width="24.81640625" style="6" customWidth="1"/>
-    <col min="6" max="6" width="14.453125" style="6" customWidth="1"/>
-    <col min="7" max="7" width="11.81640625" style="6" customWidth="1"/>
-    <col min="8" max="27" width="10.54296875" style="6" customWidth="1"/>
-    <col min="28" max="16384" width="11.26953125" style="6"/>
+    <col min="1" max="1" width="2" style="5" customWidth="1"/>
+    <col min="2" max="2" width="6.54296875" style="5" customWidth="1"/>
+    <col min="3" max="3" width="32.1796875" style="5" customWidth="1"/>
+    <col min="4" max="4" width="65.81640625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="57.6328125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="14.453125" style="5" customWidth="1"/>
+    <col min="7" max="7" width="11.81640625" style="5" customWidth="1"/>
+    <col min="8" max="27" width="10.54296875" style="5" customWidth="1"/>
+    <col min="28" max="16384" width="11.26953125" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
-      <c r="Q1" s="5"/>
-      <c r="R1" s="5"/>
-      <c r="S1" s="5"/>
-      <c r="T1" s="5"/>
-      <c r="U1" s="5"/>
-      <c r="V1" s="5"/>
-      <c r="W1" s="5"/>
-      <c r="X1" s="5"/>
-      <c r="Y1" s="5"/>
-      <c r="Z1" s="5"/>
-      <c r="AA1" s="5"/>
+      <c r="H1" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4"/>
+      <c r="R1" s="4"/>
+      <c r="S1" s="4"/>
+      <c r="T1" s="4"/>
+      <c r="U1" s="4"/>
+      <c r="V1" s="4"/>
+      <c r="W1" s="4"/>
+      <c r="X1" s="4"/>
+      <c r="Y1" s="4"/>
+      <c r="Z1" s="4"/>
+      <c r="AA1" s="4"/>
     </row>
     <row r="2" spans="1:27" ht="172.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
@@ -573,83 +700,182 @@
       <c r="B2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="F2" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="9" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:27" ht="120" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="6">
+    <row r="3" spans="1:27" ht="77.400000000000006" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="12" t="s">
+      <c r="E3" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="F3" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="H3" s="11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" ht="64.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="6"/>
+      <c r="G4" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" ht="95.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="H3" s="12" t="s">
-        <v>19</v>
+      <c r="C5" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" s="6"/>
+      <c r="G5" s="9" t="s">
+        <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F4" s="7"/>
+    <row r="6" spans="1:27" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="5">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" s="6"/>
+      <c r="G6" s="15" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="5" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F5" s="7"/>
+    <row r="7" spans="1:27" ht="81" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="5">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7" s="6"/>
+      <c r="G7" s="9" t="s">
+        <v>42</v>
+      </c>
     </row>
-    <row r="6" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F6" s="7"/>
+    <row r="8" spans="1:27" ht="75.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="5">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="F8" s="6"/>
+      <c r="G8" s="9" t="s">
+        <v>41</v>
+      </c>
     </row>
-    <row r="7" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F7" s="7"/>
-    </row>
-    <row r="8" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F8" s="7"/>
-    </row>
-    <row r="9" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F9" s="7"/>
+    <row r="9" spans="1:27" ht="76.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
+        <v>8</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="F9" s="6"/>
     </row>
     <row r="10" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F10" s="7"/>
+      <c r="F10" s="6"/>
     </row>
     <row r="11" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F11" s="7"/>
+      <c r="F11" s="6"/>
     </row>
     <row r="12" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F12" s="7"/>
+      <c r="F12" s="6"/>
     </row>
     <row r="13" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F13" s="7"/>
+      <c r="F13" s="6"/>
     </row>
     <row r="14" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F14" s="7"/>
+      <c r="F14" s="6"/>
     </row>
     <row r="15" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F15" s="7"/>
+      <c r="F15" s="6"/>
     </row>
     <row r="16" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1640,8 +1866,13 @@
   <hyperlinks>
     <hyperlink ref="G2" r:id="rId1"/>
     <hyperlink ref="G3" r:id="rId2"/>
+    <hyperlink ref="G4" r:id="rId3"/>
+    <hyperlink ref="G5" r:id="rId4"/>
+    <hyperlink ref="G6" r:id="rId5"/>
+    <hyperlink ref="G8" r:id="rId6"/>
+    <hyperlink ref="G7" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape" r:id="rId3"/>
+  <pageSetup orientation="landscape" r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
rapport de plusieurs bug
eurrer d'écriture pour la balise  <!DOCTYPE html> (2récurence sur la page Index.html et Page2.html)
La balise meta "keywords" est obsolète et ne devrait pas être utilisée(2récurence sur la page Index.html et Page2.html)
Il y a une balise <li> inutile à la ligne 50
eurrer d'écriture pour la balise                   <html lang="Default">(2récurence sur la page Index.html et Page2.html)
Pas de titre (2récurence sur la page Index.html et Page2.html)
/ ajouté en trop (13récurence sur la page Index.html et Page2.html)
eurre avec la balise from
média obsolète min-device-width (2récurence dans le style.css)
média obsolète max-device-width (2récurence dans le style.css)

Manque sitemap
Nom page 2
ajout de meta name robots
Balise sémantique
script unitile
<meta name="description" content=""> vide
Defer
CDN
changement de place <link rel="stylesheet" type="text/css" href="style.css">
utilise des Images pour faire du texte
taille du texte
Mauvais hierarchie des titres
</commit_message>
<xml_diff>
--- a/Modèle-audit-SEO.xlsx
+++ b/Modèle-audit-SEO.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="80">
   <si>
     <t>Catégorie</t>
   </si>
@@ -300,12 +300,61 @@
     <t>utiliser les balises sémantique ( A FAIRE)</t>
   </si>
   <si>
-    <t xml:space="preserve">    Utilisez des balises d'en-tête (H1, H2, etc.) pour structurer votre contenu et aider les moteurs de recherche à comprendre la hiérarchie de votre contenu.
-    Utilisez un sitemap pour aider les moteurs de recherche à explorer le site.
-    Utilisez des balises canoniques pour éviter les doublons de contenu.
-    Utilisez la balise "meta name="robots" content="index, follow"" pour indiquer aux moteurs de recherche de l'indexer et de suivre les liens.
-    Utilisez des noms de fichiers descriptifs pour vos pages.
-    Utilisez des balises sémantiques pour améliorer l'accessibilité et la compréhension de votre contenu par les moteurs de recherche.</t>
+    <t xml:space="preserve"> Google Maps n'est pas utilisé sur le site, il n'est pas nécessaire d'inclure le fichier gmaps.js. Cela peut ralentir le temps de chargement du site et augmenter la taille de votre code HTML pour rien. Il est donc préférable de supprimer cette ligne de code de le fichier HTML.</t>
+  </si>
+  <si>
+    <t>supprimer &lt;script src="./js/gmaps.js"&gt;&lt;/script&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">script unitile </t>
+  </si>
+  <si>
+    <t>&lt;meta name="description" content=""&gt; vide</t>
+  </si>
+  <si>
+    <t>Defer</t>
+  </si>
+  <si>
+    <t>Lorsque on utilise "defer" dans un script, cela signifie que le script ne sera pas chargé ou exécuté avant que le reste de la page HTML n'ait été chargé. Cela peut aider à améliorer les performances de votre site web car les scripts ne bloquent pas le chargement de la page.</t>
+  </si>
+  <si>
+    <t>utiliser defer dans les script</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CDN </t>
+  </si>
+  <si>
+    <t xml:space="preserve">changement de place &lt;link rel="stylesheet" type="text/css" href="style.css"&gt; </t>
+  </si>
+  <si>
+    <t>Il est recommandé de placer le fichier CSS en dernier dans la liste de chargement pour éviter que des styles ne soient remplacés ou ignorés par des feuilles de style chargées ultérieurement. Cela permet également de s'assurer que les styles personnalisés sont appliqués après ceux définis par les feuilles de style de bibliothèques ou de frameworks utilisés.</t>
+  </si>
+  <si>
+    <t>placer le fichier CSS en dernier dans la liste</t>
+  </si>
+  <si>
+    <t xml:space="preserve">utilise des Images pour faire du texte </t>
+  </si>
+  <si>
+    <t>Il est préférable d'utiliser des balises de texte pour les titres et les paragraphes plutôt que d'utiliser des images pour afficher du texte. Les images ne sont pas accessibles aux utilisateurs d'écran et ne peuvent pas être indexées par les moteurs de recherche, ce qui peut impacter le référencement. Il est préférable d'utiliser des styles CSS pour personnaliser l'apparence du texte plutôt que d'utiliser des images.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">remplacer les images par du texte </t>
+  </si>
+  <si>
+    <t>Il est important d'utiliser une taille de police adéquate pour rendre le contenu du votre site facile à lire et à comprendre pour tous les utilisateurs. Utiliser des tailles de police en rem permet de garantir que la taille de police est proportionnelle à la taille de l'écran de l'utilisateur, garantissant ainsi une expérience utilisateur optimale sur tous les appareils. Cela permet également d'améliorer l'accessibilité pour les personnes ayant des difficultés de vision.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">taille du texte </t>
+  </si>
+  <si>
+    <t xml:space="preserve">mettre en REM </t>
+  </si>
+  <si>
+    <t>Constant existe pas normal c'est ENV,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mauvais hierarchie des titres </t>
   </si>
 </sst>
 </file>
@@ -420,7 +469,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="3"/>
+        <fgColor rgb="FFC00000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -445,7 +494,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -492,16 +541,13 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -720,10 +766,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA1000"/>
+  <dimension ref="A1:AA999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.26953125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -987,101 +1033,173 @@
       <c r="D11" s="14" t="s">
         <v>48</v>
       </c>
+      <c r="E11" s="5" t="s">
+        <v>78</v>
+      </c>
       <c r="F11" s="6"/>
     </row>
-    <row r="12" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="16"/>
-      <c r="B12" s="17" t="s">
+    <row r="12" spans="1:27" ht="83.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="5">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="16"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="16"/>
-    </row>
-    <row r="13" spans="1:27" ht="83.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C12" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F12" s="6"/>
+      <c r="G12" s="9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27" ht="84.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
-        <v>11</v>
-      </c>
-      <c r="B13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="E13" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="F13" s="6"/>
+    </row>
+    <row r="14" spans="1:27" ht="55.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="5">
+        <v>13</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F14" s="6"/>
+    </row>
+    <row r="15" spans="1:27" ht="85.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="5">
+        <v>14</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27" ht="67.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="5">
+        <v>15</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="35.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="5">
+        <v>16</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="64.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="5">
+        <v>17</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D18" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="5">
+        <v>18</v>
+      </c>
+      <c r="C19" s="17" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="75.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="5">
+        <v>19</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="58.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="5">
         <v>20</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D13" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="F13" s="6"/>
-      <c r="G13" s="9" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="14" spans="1:27" ht="84.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="5">
-        <v>12</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D14" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="E14" s="19" t="s">
-        <v>56</v>
-      </c>
-      <c r="F14" s="6"/>
-    </row>
-    <row r="15" spans="1:27" ht="55.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="5">
-        <v>13</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D15" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F15" s="6"/>
-    </row>
-    <row r="16" spans="1:27" ht="85.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C16" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="D16" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="17" spans="4:4" ht="131.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D17" s="11" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="18" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="19" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="20" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="22" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="C21" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="D21" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="97.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C22" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="D22" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="36.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C23" s="14" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2049,7 +2167,6 @@
     <row r="997" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G2" r:id="rId1"/>
@@ -2061,7 +2178,7 @@
     <hyperlink ref="G7" r:id="rId7"/>
     <hyperlink ref="G9" r:id="rId8"/>
     <hyperlink ref="G10" r:id="rId9"/>
-    <hyperlink ref="G13" r:id="rId10"/>
+    <hyperlink ref="G12" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId11"/>

</xml_diff>

<commit_message>
Amélioration d'accessibilité du texte,Defer et CDN
</commit_message>
<xml_diff>
--- a/Modèle-audit-SEO.xlsx
+++ b/Modèle-audit-SEO.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="88">
   <si>
     <t>Catégorie</t>
   </si>
@@ -351,32 +351,41 @@
     <t xml:space="preserve">Image trop lourd </t>
   </si>
   <si>
-    <t xml:space="preserve"> &lt;!-- &lt;script src="https://code.jquery.com/jquery-2.1.0.js" defer&gt;&lt;/script&gt;
- &lt;script src="https://maxcdn.bootstrapcdn.com/bootstrap/3.3.7/js/bootstrap.js" defer&gt;&lt;/script&gt;
- &lt;script src="https://cdnjs.cloudflare.com/ajax/libs/blocs.js/1.0.0/blocs.js" defer&gt;&lt;/script&gt;
- &lt;script src="https://cdnjs.cloudflare.com/ajax/libs/jquery.touchswipe/1.6.18/jquery.touchSwipe.js" defer&gt;&lt;/script&gt; --&gt;</t>
-  </si>
-  <si>
     <t xml:space="preserve">Pratique de Backhat </t>
   </si>
   <si>
     <t>Les pratiques black hat visent à manipuler les résultats de recherche en utilisant des techniques illégales. L'ajout de partenaires bidon est l'une de ces techniques qui peut causer des dommages à long terme au référencement d'un site. Il est préférable d'éviter ces pratiques.</t>
   </si>
   <si>
-    <t xml:space="preserve">supréssion du code abusif </t>
-  </si>
-  <si>
     <t xml:space="preserve">Amélioration des Alt sur les Images </t>
   </si>
   <si>
     <t>Les alt sont des attributs dans les balises img qui décrivent une image en cas où elle ne peut pas être chargée. Il est important d'utiliser des alt pertinents car ils aident les utilisateurs d'écran et les moteurs de recherche à comprendre le contenu de l'image. Cela peut aider à améliorer l'accessibilité et le référencement du site.</t>
+  </si>
+  <si>
+    <t>supréssion du code abusif avec les annuaires et les moot en tout petit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">le responsive est mal fait </t>
+  </si>
+  <si>
+    <t xml:space="preserve">c good intgrity </t>
+  </si>
+  <si>
+    <t>les couleurs du texte</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mimifier </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Core web vals </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -456,8 +465,20 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="9"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFFC000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -494,6 +515,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -515,7 +542,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -538,9 +565,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -579,6 +603,30 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -799,7 +847,7 @@
   <dimension ref="A1:AA998"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.26953125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -816,7 +864,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="12" t="s">
         <v>6</v>
       </c>
       <c r="B1" s="3" t="s">
@@ -837,7 +885,7 @@
       <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="H1" s="11" t="s">
         <v>17</v>
       </c>
       <c r="I1" s="4"/>
@@ -867,21 +915,22 @@
       <c r="B2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="24" t="s">
         <v>11</v>
       </c>
+      <c r="H2" s="23"/>
     </row>
     <row r="3" spans="1:27" ht="77.400000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
@@ -893,19 +942,19 @@
       <c r="C3" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="G3" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="11" t="s">
+      <c r="H3" s="10" t="s">
         <v>18</v>
       </c>
     </row>
@@ -919,14 +968,14 @@
       <c r="C4" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="E4" s="10" t="s">
         <v>23</v>
       </c>
       <c r="F4" s="6"/>
-      <c r="G4" s="9" t="s">
+      <c r="G4" s="8" t="s">
         <v>24</v>
       </c>
     </row>
@@ -937,17 +986,17 @@
       <c r="B5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="14" t="s">
+      <c r="E5" s="13" t="s">
         <v>26</v>
       </c>
       <c r="F5" s="6"/>
-      <c r="G5" s="9" t="s">
+      <c r="G5" s="8" t="s">
         <v>27</v>
       </c>
     </row>
@@ -958,17 +1007,17 @@
       <c r="B6" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="D6" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="E6" s="13" t="s">
         <v>29</v>
       </c>
       <c r="F6" s="6"/>
-      <c r="G6" s="15" t="s">
+      <c r="G6" s="14" t="s">
         <v>30</v>
       </c>
     </row>
@@ -979,17 +1028,17 @@
       <c r="B7" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="D7" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="E7" s="11" t="s">
+      <c r="E7" s="10" t="s">
         <v>33</v>
       </c>
       <c r="F7" s="6"/>
-      <c r="G7" s="9" t="s">
+      <c r="G7" s="8" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1003,14 +1052,14 @@
       <c r="C8" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="D8" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="E8" s="11" t="s">
+      <c r="E8" s="10" t="s">
         <v>37</v>
       </c>
       <c r="F8" s="6"/>
-      <c r="G8" s="9" t="s">
+      <c r="G8" s="8" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1018,20 +1067,20 @@
       <c r="A9" s="5">
         <v>8</v>
       </c>
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="C9" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="D9" s="14" t="s">
+      <c r="D9" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="E9" s="14" t="s">
+      <c r="E9" s="13" t="s">
         <v>46</v>
       </c>
       <c r="F9" s="6"/>
-      <c r="G9" s="9" t="s">
+      <c r="G9" s="8" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1039,20 +1088,20 @@
       <c r="A10" s="5">
         <v>9</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="14" t="s">
+      <c r="C10" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="D10" s="14" t="s">
+      <c r="D10" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="E10" s="14" t="s">
+      <c r="E10" s="13" t="s">
         <v>46</v>
       </c>
       <c r="F10" s="6"/>
-      <c r="G10" s="9" t="s">
+      <c r="G10" s="8" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1060,7 +1109,7 @@
       <c r="A11" s="5">
         <v>10</v>
       </c>
-      <c r="D11" s="14" t="s">
+      <c r="D11" s="13" t="s">
         <v>48</v>
       </c>
       <c r="E11" s="5" t="s">
@@ -1078,14 +1127,14 @@
       <c r="C12" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D12" s="11" t="s">
+      <c r="D12" s="10" t="s">
         <v>50</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>51</v>
       </c>
       <c r="F12" s="6"/>
-      <c r="G12" s="9" t="s">
+      <c r="G12" s="24" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1096,10 +1145,10 @@
       <c r="C13" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="D13" s="11" t="s">
+      <c r="D13" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="E13" s="16" t="s">
+      <c r="E13" s="15" t="s">
         <v>56</v>
       </c>
       <c r="F13" s="6"/>
@@ -1111,7 +1160,7 @@
       <c r="C14" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D14" s="11" t="s">
+      <c r="D14" s="10" t="s">
         <v>54</v>
       </c>
       <c r="E14" s="1" t="s">
@@ -1126,13 +1175,13 @@
       <c r="C15" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="D15" s="11" t="s">
+      <c r="D15" s="10" t="s">
         <v>59</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="F15" s="19"/>
+      <c r="F15" s="18"/>
     </row>
     <row r="16" spans="1:27" ht="67.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
@@ -1141,126 +1190,147 @@
       <c r="C16" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="D16" s="11" t="s">
+      <c r="D16" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="E16" s="5" t="s">
+      <c r="E16" s="22" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" ht="35.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F16" s="21"/>
+      <c r="G16" s="23"/>
+    </row>
+    <row r="17" spans="1:7" ht="35.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>16</v>
       </c>
-      <c r="C17" s="14" t="s">
+      <c r="C17" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="F17" s="19"/>
-    </row>
-    <row r="18" spans="1:6" ht="64.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F17" s="18"/>
+    </row>
+    <row r="18" spans="1:7" ht="64.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>17</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="D18" s="14" t="s">
+      <c r="D18" s="13" t="s">
         <v>66</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="F18" s="21"/>
-    </row>
-    <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F18" s="20"/>
+    </row>
+    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>18</v>
       </c>
-      <c r="C19" s="17" t="s">
+      <c r="C19" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="D19" s="14" t="s">
-        <v>78</v>
-      </c>
-      <c r="F19" s="21"/>
-    </row>
-    <row r="20" spans="1:6" ht="58.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D19" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="F19" s="20"/>
+    </row>
+    <row r="20" spans="1:7" ht="58.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>20</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="D20" s="18" t="s">
+      <c r="D20" s="17" t="s">
         <v>70</v>
       </c>
       <c r="E20" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="F20" s="19"/>
-    </row>
-    <row r="21" spans="1:6" ht="97.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F20" s="18"/>
+    </row>
+    <row r="21" spans="1:7" ht="97.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>21</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="D21" s="14" t="s">
+      <c r="D21" s="13" t="s">
         <v>72</v>
       </c>
       <c r="E21" s="5" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="36.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="36.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>22</v>
       </c>
-      <c r="C22" s="20" t="s">
+      <c r="C22" s="19" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F22" s="18"/>
+    </row>
+    <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
         <v>23</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="F23" s="19"/>
-    </row>
-    <row r="24" spans="1:6" ht="46.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F23" s="18"/>
+    </row>
+    <row r="24" spans="1:7" ht="46.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
         <v>2</v>
       </c>
       <c r="C24" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="D24" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="D24" s="20" t="s">
+      <c r="E24" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="F24" s="18"/>
+    </row>
+    <row r="25" spans="1:7" ht="47.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C25" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="E24" s="5" t="s">
+      <c r="D25" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="F24" s="19"/>
-    </row>
-    <row r="25" spans="1:6" ht="47.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C25" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="D25" s="14" t="s">
+      <c r="F25" s="18"/>
+    </row>
+    <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C26" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="F25" s="19"/>
-    </row>
-    <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="F26" s="18"/>
+    </row>
+    <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C27" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="G27" s="25"/>
+    </row>
+    <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C28" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C29" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
correction / sur image et correction des bug de la vielle
</commit_message>
<xml_diff>
--- a/Modèle-audit-SEO.xlsx
+++ b/Modèle-audit-SEO.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="121">
   <si>
     <t>Catégorie</t>
   </si>
@@ -405,6 +405,9 @@
       &lt;/label&gt;
       &lt;input id="email" class="form-control" type="email" required=""&gt;
      &lt;div class="help-block"&gt;&lt;/div&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Boostrap et jequery sécurité </t>
   </si>
 </sst>
 </file>
@@ -878,8 +881,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA998"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.23046875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1498,7 +1501,11 @@
         <v>119</v>
       </c>
     </row>
-    <row r="41" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="41" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C41" s="5" t="s">
+        <v>120</v>
+      </c>
+    </row>
     <row r="42" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="43" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="44" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>

</xml_diff>